<commit_message>
Updated Tree Excel Sheet
</commit_message>
<xml_diff>
--- a/assets/Map/Tree Unit Sprite.xlsx
+++ b/assets/Map/Tree Unit Sprite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Action</t>
   </si>
@@ -426,7 +426,7 @@
   <dimension ref="A2:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B14"/>
+      <selection activeCell="H3" sqref="H3:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -468,20 +468,36 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
       <c r="F3" s="3"/>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
         <f>A3+1</f>
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
       <c r="F4" s="3"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
@@ -489,24 +505,27 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
       <c r="F5" s="3"/>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
         <f t="shared" ref="A6:A50" si="0">A5+1</f>
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:10">
@@ -514,21 +533,16 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="F7" s="3"/>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -536,45 +550,23 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="F8" s="3"/>
-      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="F9" s="3"/>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:10">
@@ -582,34 +574,15 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="F11" s="3"/>
-      <c r="H11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
+      <c r="B12" s="4"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:10">
@@ -617,12 +590,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
+      <c r="B13" s="4"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:10">
@@ -630,12 +598,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
+      <c r="B14" s="4"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:10">
@@ -644,9 +607,6 @@
         <v>12</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:10">
@@ -655,9 +615,6 @@
         <v>13</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6">
@@ -666,9 +623,6 @@
         <v>14</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6">
@@ -677,9 +631,6 @@
         <v>15</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6">
@@ -688,9 +639,6 @@
         <v>16</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6">
@@ -699,9 +647,6 @@
         <v>17</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6">
@@ -710,9 +655,6 @@
         <v>18</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6">
@@ -721,9 +663,6 @@
         <v>19</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" t="s">
-        <v>16</v>
-      </c>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6">
@@ -732,9 +671,6 @@
         <v>20</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6">
@@ -743,9 +679,6 @@
         <v>21</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6">
@@ -754,9 +687,6 @@
         <v>22</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6">
@@ -765,9 +695,6 @@
         <v>23</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6">
@@ -775,215 +702,143 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+    </row>
+    <row r="33" spans="1:1">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+    </row>
+    <row r="34" spans="1:1">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="C35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+    </row>
+    <row r="36" spans="1:1">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="C36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+    </row>
+    <row r="37" spans="1:1">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="C37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+    </row>
+    <row r="38" spans="1:1">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="C38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+    </row>
+    <row r="39" spans="1:1">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+    </row>
+    <row r="40" spans="1:1">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="C40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+    </row>
+    <row r="41" spans="1:1">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="C41" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+    </row>
+    <row r="42" spans="1:1">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="C42" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+    </row>
+    <row r="43" spans="1:1">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+    </row>
+    <row r="44" spans="1:1">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+    </row>
+    <row r="45" spans="1:1">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="C45" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+    </row>
+    <row r="46" spans="1:1">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+    </row>
+    <row r="47" spans="1:1">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="C47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+    </row>
+    <row r="48" spans="1:1">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="C48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+    </row>
+    <row r="49" spans="1:1">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="C49" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+    </row>
+    <row r="50" spans="1:1">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>47</v>
-      </c>
-      <c r="C50" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>